<commit_message>
MAJ journal d'apprentissage à date 24/01/19 18h50
</commit_message>
<xml_diff>
--- a/Journal d'apprentissage.xlsx
+++ b/Journal d'apprentissage.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://axa365-my.sharepoint.com/personal/gregory_lescroel_axa_fr/Documents/Bureau/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{76439ADF-2CD5-410A-BEC0-278868A2B60A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7100" xr2:uid="{2E869303-75E8-49F4-8BE9-372D448FD523}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$D$127</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -48,16 +42,28 @@
 Je dois réaliser les tâches "administratives" du premier projet avant de pouvoir passer au sujet</t>
   </si>
   <si>
-    <t>Objectifs : me débarrasser asap des tâches administratives pour pouvoir démarrer !</t>
+    <t>Objectifs : me débarrasser asap des tâches administratives pour pouvoir démarrer !
+14h20 : fichiers du projet 1 envoyés à Stéphane Didier pour validation ! --&gt; je peux passer au projet 2 !</t>
+  </si>
+  <si>
+    <t>J'ai passé la journée sur le cours Git / GitHub et la termine par l'activité de la seconde partie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -72,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -111,6 +117,43 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -120,22 +163,50 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -143,74 +214,41 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,61 +555,67 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76772A8D-EDC5-47F2-AFC6-84FD7EFEAAE3}">
-  <dimension ref="B1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="103" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="1" t="s">
+    <row r="1" spans="2:3" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="9" t="s">
+    <row r="3" spans="2:3" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="8">
+    <row r="4" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
         <v>43486</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="6">
+    <row r="5" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
         <v>43487</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="7">
+    <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
         <v>43488</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="7" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
+        <v>43489</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>